<commit_message>
added excel writer methods
</commit_message>
<xml_diff>
--- a/ExcelData/a.xlsx
+++ b/ExcelData/a.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyStoreProject\ExcelData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAD277E-DAF4-4AB1-9EE0-103992E3D3FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A61F12B3-C1ED-45B0-8F17-1DE7090F8A97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22464" windowHeight="7284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +11,12 @@
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Jyo</t>
   </si>
@@ -37,19 +33,29 @@
     <t>Password</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validation Status</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,41 +402,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>

</xml_diff>